<commit_message>
refactor: add numbers uc detailled model
</commit_message>
<xml_diff>
--- a/1-exercices/ressources/uc_details.xlsx
+++ b/1-exercices/ressources/uc_details.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\formations\coderbase\m2i\poe-javafull-05062023\4-poo-uml\1-exercices\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFCB8A3-186A-4FD8-A1F3-EFEC6345569E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDC378A-3B8E-4D49-9D6E-2465819A2517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30610" yWindow="-60" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30610" yWindow="-60" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Consulter produit" sheetId="1" r:id="rId1"/>
-    <sheet name="Exemple" sheetId="2" r:id="rId2"/>
+    <sheet name="Exemple" sheetId="2" r:id="rId1"/>
+    <sheet name="Modèle" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Nom UC</t>
   </si>
@@ -66,34 +66,6 @@
     <t>Banque</t>
   </si>
   <si>
-    <t>Demande à effectuer une commande</t>
-  </si>
-  <si>
-    <t>Demande de saisir une adresse de livraison et de valider</t>
-  </si>
-  <si>
-    <t>Saisi l'adresse de livraison et valide</t>
-  </si>
-  <si>
-    <t>Vérifie l'adresse de livraison</t>
-  </si>
-  <si>
-    <t>Demande de saisir les informations du moyen de paiement et de valider</t>
-  </si>
-  <si>
-    <t>Saisi les informations de paiement et valide</t>
-  </si>
-  <si>
-    <t>Demande de réaliser la transaction à la banque</t>
-  </si>
-  <si>
-    <t>Vérifie les informations 
-et retourne une réponse favorable au système</t>
-  </si>
-  <si>
-    <t>Affiche un message de succès de la commande</t>
-  </si>
-  <si>
     <t>Scenario alternatif 1 : adresse de livraison incorrecte</t>
   </si>
   <si>
@@ -126,10 +98,47 @@
 vers la "page" de contact</t>
   </si>
   <si>
-    <t>Pré-condtions</t>
-  </si>
-  <si>
-    <t>Post-conditions</t>
+    <t>Autre Système</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario alternatif 1 : </t>
+  </si>
+  <si>
+    <t>Scenario alternatif 2 :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario alternatif 2 : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario d'erreur : </t>
+  </si>
+  <si>
+    <t>1. Demande à effectuer une commande</t>
+  </si>
+  <si>
+    <t>2.Demande de saisir une adresse de livraison et de valider</t>
+  </si>
+  <si>
+    <t>3. Saisi l'adresse de livraison et valide</t>
+  </si>
+  <si>
+    <t>4.Vérifie l'adresse de livraison</t>
+  </si>
+  <si>
+    <t>5. Demande de saisir les informations du moyen de paiement et de valider</t>
+  </si>
+  <si>
+    <t>6. Saisi les informations de paiement et valide</t>
+  </si>
+  <si>
+    <t>7.Demande de réaliser la transaction à la banque</t>
+  </si>
+  <si>
+    <t>8. Vérifie les informations 
+et retourne une réponse favorable au système</t>
+  </si>
+  <si>
+    <t>9. Affiche un message de succès de la commande</t>
   </si>
 </sst>
 </file>
@@ -546,83 +555,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -630,8 +562,8 @@
   </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -709,7 +641,7 @@
     <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -718,14 +650,14 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="5" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -734,7 +666,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -742,14 +674,14 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="5" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -758,7 +690,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -767,14 +699,14 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -786,23 +718,23 @@
     </row>
     <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -814,13 +746,13 @@
     </row>
     <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -832,12 +764,197 @@
     </row>
     <row r="22" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="49" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF8BE59-B86F-4A5E-BDE1-77D120355DFA}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="66.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="124.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="1"/>
     </row>
   </sheetData>

</xml_diff>